<commit_message>
correccion spinners imports y restauracion boton excel auditoria
</commit_message>
<xml_diff>
--- a/frontend/web/uploads/Customer.xlsx
+++ b/frontend/web/uploads/Customer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://agcompany-my.sharepoint.com/personal/romina_oliverio_corteva_com/Documents/CORTEVA/2 - Demand Analyst/PODIUM/Customers/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{4FAF78C1-1510-44EA-B2DF-5E3FDC4E9934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E9120F1-C8CE-457B-859D-F654AEAC69B2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{30B3575F-48A3-41F4-90E4-76768E9F193C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="397" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3481,8 +3481,8 @@
   <sheetPr codeName="SAPBEXqueries"/>
   <dimension ref="A1:M683"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A660" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="A681" sqref="A681"/>
+    <sheetView tabSelected="1" topLeftCell="I134" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="M134" sqref="M134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.54296875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -32045,22 +32045,32 @@
     <hyperlink ref="G681" r:id="rId596" display="mailto:marcos.fiol@brevant.com" xr:uid="{4368A9EC-AFAA-478E-9A61-9C612AD400F4}"/>
     <hyperlink ref="J681" r:id="rId597" xr:uid="{51E25035-B6FB-49E6-8562-F3201B0FE2FD}"/>
     <hyperlink ref="M681" r:id="rId598" xr:uid="{7028E102-F2C6-48FE-8467-A14BB59ED0DA}"/>
+    <hyperlink ref="G375" r:id="rId599" xr:uid="{99F79578-F616-4BA3-9E10-D1060B2C1A9F}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="256" orientation="portrait" r:id="rId599"/>
+  <pageSetup paperSize="256" orientation="portrait" r:id="rId600"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Calibri"&amp;11&amp;K000000&amp;"Calibri"&amp;11&amp;K000000DOW RESTRICTED_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000---Internal Use---</oddFooter>
   </headerFooter>
   <customProperties>
-    <customPr name="_pios_id" r:id="rId600"/>
-    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId601"/>
-    <customPr name="FPMExcelClientCellBasedFunctionStatus" r:id="rId602"/>
-    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId603"/>
+    <customPr name="_pios_id" r:id="rId601"/>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId602"/>
+    <customPr name="FPMExcelClientCellBasedFunctionStatus" r:id="rId603"/>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId604"/>
   </customProperties>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C67116C3FE43E40BC2044BD15494AB9" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="872b91e4d0b87627fc35dd2b027aac34">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6e991132-a773-4509-b2e6-2c1b1f1c0078" xmlns:ns3="6568133d-d520-40b4-aa9b-b3297c4de197" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a98e141f55e226a86617e6567c885c0b" ns2:_="" ns3:_="">
     <xsd:import namespace="6e991132-a773-4509-b2e6-2c1b1f1c0078"/>
@@ -32239,15 +32249,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -32255,6 +32256,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{234DF6E0-189F-4E45-8857-EAF273DD9FAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07917689-C5F2-4279-A8AD-20854CD3566A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32269,14 +32278,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{234DF6E0-189F-4E45-8857-EAF273DD9FAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>